<commit_message>
Updated progress and tracking documents
</commit_message>
<xml_diff>
--- a/Notes/Progress & tracking/Meetings - attendance.xlsx
+++ b/Notes/Progress & tracking/Meetings - attendance.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Development\Uni\Robot Programming\workspace\Autonomous_Warehouse_Project\Notes\Progress &amp; tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736D1388-C1F9-4CF2-A6CA-1DF1B47A8D15}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{32695725-CAA4-477E-93D3-CB15806689B3}"/>
   </bookViews>
@@ -250,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -997,7 +998,7 @@
   <dimension ref="B4:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,11 +1096,11 @@
       <c r="H6" s="24">
         <v>43171</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>13</v>
+      <c r="I6" s="24">
+        <v>43172</v>
+      </c>
+      <c r="J6" s="24">
+        <v>43174</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>13</v>
@@ -1142,17 +1143,21 @@
       <c r="H7" s="5">
         <v>1</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>1</v>
+      </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5">
         <f>COUNTIF(C7:L7,"=1")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N7" s="4">
         <f>COUNTIF(C7:L7,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
@@ -1177,13 +1182,17 @@
       <c r="H8" s="5">
         <v>1</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1</v>
+      </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="9">
         <f t="shared" ref="M8:M16" si="0">COUNTIF(C8:L8,"=1")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N8" s="8">
         <f t="shared" ref="N8:N16" si="1">COUNTIF(C8:L8,0)</f>
@@ -1212,13 +1221,17 @@
       <c r="H9" s="5">
         <v>1</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1</v>
+      </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N9" s="8">
         <f t="shared" si="1"/>
@@ -1247,17 +1260,21 @@
       <c r="H10" s="5">
         <v>1</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1</v>
+      </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N10" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
@@ -1282,13 +1299,17 @@
       <c r="H11" s="5">
         <v>1</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N11" s="8">
         <f t="shared" si="1"/>
@@ -1317,13 +1338,17 @@
       <c r="H12" s="5">
         <v>1</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1</v>
+      </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N12" s="8">
         <f t="shared" si="1"/>
@@ -1352,13 +1377,17 @@
       <c r="H13" s="5">
         <v>1</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+      <c r="I13" s="5">
+        <v>1</v>
+      </c>
+      <c r="J13" s="5">
+        <v>1</v>
+      </c>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N13" s="8">
         <f t="shared" si="1"/>
@@ -1387,17 +1416,21 @@
       <c r="H14" s="5">
         <v>1</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="I14" s="5">
+        <v>1</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N14" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
@@ -1422,13 +1455,17 @@
       <c r="H15" s="5">
         <v>1</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="I15" s="5">
+        <v>1</v>
+      </c>
+      <c r="J15" s="5">
+        <v>1</v>
+      </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N15" s="8">
         <f t="shared" si="1"/>
@@ -1457,13 +1494,17 @@
       <c r="H16" s="5">
         <v>1</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="I16" s="5">
+        <v>1</v>
+      </c>
+      <c r="J16" s="5">
+        <v>1</v>
+      </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N16" s="1">
         <f t="shared" si="1"/>
@@ -1500,11 +1541,11 @@
       </c>
       <c r="I17" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J17" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K17" s="11">
         <f t="shared" si="2"/>

</xml_diff>